<commit_message>
Added input file for ESAC1A.
</commit_message>
<xml_diff>
--- a/andes/cases/ieee14/ieee14_esac1a.xlsx
+++ b/andes/cases/ieee14/ieee14_esac1a.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jinningwang/Documents/work/andes/andes/cases/ieee14/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{21C90B1C-9DB6-9644-8FA2-E3ACFB5E0454}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C2CE0657-98B6-8645-928D-CF5CF7E83EB5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28800" yWindow="500" windowWidth="27320" windowHeight="19980" activeTab="12" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="19200" yWindow="500" windowWidth="19200" windowHeight="21100" firstSheet="4" activeTab="12" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Toggler" sheetId="1" r:id="rId1"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="355" uniqueCount="172">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="364" uniqueCount="180">
   <si>
     <t>idx</t>
   </si>
@@ -549,6 +549,30 @@
   </si>
   <si>
     <t>Switch</t>
+  </si>
+  <si>
+    <t>VAMAX</t>
+  </si>
+  <si>
+    <t>VAMIN</t>
+  </si>
+  <si>
+    <t>E1</t>
+  </si>
+  <si>
+    <t>SE1</t>
+  </si>
+  <si>
+    <t>E2</t>
+  </si>
+  <si>
+    <t>SE2</t>
+  </si>
+  <si>
+    <t>KE</t>
+  </si>
+  <si>
+    <t>KD</t>
   </si>
 </sst>
 </file>
@@ -618,12 +642,15 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
   </cellXfs>
@@ -1772,16 +1799,16 @@
 
 <file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0C00-000000000000}">
-  <dimension ref="A1:P2"/>
+  <dimension ref="A1:Y2"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D1" zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="N1" zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="M2" sqref="M2"/>
+      <selection pane="bottomLeft" activeCell="T10" sqref="T10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>6</v>
       </c>
@@ -1807,31 +1834,58 @@
         <v>140</v>
       </c>
       <c r="I1" s="2" t="s">
+        <v>172</v>
+      </c>
+      <c r="J1" s="2" t="s">
+        <v>173</v>
+      </c>
+      <c r="K1" s="2" t="s">
         <v>142</v>
       </c>
-      <c r="J1" s="2" t="s">
+      <c r="L1" s="2" t="s">
         <v>143</v>
       </c>
-      <c r="K1" s="2" t="s">
+      <c r="M1" s="2" t="s">
         <v>144</v>
       </c>
-      <c r="L1" s="2" t="s">
+      <c r="N1" s="2" t="s">
         <v>145</v>
       </c>
-      <c r="M1" s="2" t="s">
+      <c r="O1" s="2" t="s">
         <v>170</v>
       </c>
-      <c r="N1" s="2" t="s">
+      <c r="P1" s="1" t="s">
+        <v>174</v>
+      </c>
+      <c r="Q1" s="1" t="s">
+        <v>175</v>
+      </c>
+      <c r="R1" s="1" t="s">
+        <v>176</v>
+      </c>
+      <c r="S1" s="1" t="s">
+        <v>177</v>
+      </c>
+      <c r="T1" s="3" t="s">
+        <v>179</v>
+      </c>
+      <c r="U1" s="3" t="s">
+        <v>146</v>
+      </c>
+      <c r="V1" s="3" t="s">
+        <v>178</v>
+      </c>
+      <c r="W1" s="2" t="s">
         <v>147</v>
       </c>
-      <c r="O1" s="2" t="s">
+      <c r="X1" s="2" t="s">
         <v>148</v>
       </c>
-      <c r="P1" s="2" t="s">
+      <c r="Y1" s="2" t="s">
         <v>171</v>
       </c>
     </row>
-    <row r="2" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A2" s="1">
         <v>0</v>
       </c>

</xml_diff>